<commit_message>
added a few lines to later generate a histogram
</commit_message>
<xml_diff>
--- a/Pearsons_CC/Python_Code/1test.xlsx
+++ b/Pearsons_CC/Python_Code/1test.xlsx
@@ -1,16 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28410"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eldabaghr/Bioinf/Pearsons_CC/Python_Code/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9860" yWindow="0" windowWidth="25360" windowHeight="18780" tabRatio="500"/>
+    <workbookView xWindow="9860" yWindow="460" windowWidth="25360" windowHeight="18780" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -19,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>YCL020W</t>
   </si>
@@ -79,6 +87,45 @@
   </si>
   <si>
     <t>PST2</t>
+  </si>
+  <si>
+    <t>gene</t>
+  </si>
+  <si>
+    <t>exp1</t>
+  </si>
+  <si>
+    <t>exp2</t>
+  </si>
+  <si>
+    <t>exp3</t>
+  </si>
+  <si>
+    <t>exp4</t>
+  </si>
+  <si>
+    <t>exp5</t>
+  </si>
+  <si>
+    <t>exp6</t>
+  </si>
+  <si>
+    <t>exp7</t>
+  </si>
+  <si>
+    <t>exp8</t>
+  </si>
+  <si>
+    <t>exp9</t>
+  </si>
+  <si>
+    <t>exp10</t>
+  </si>
+  <si>
+    <t>exp11</t>
+  </si>
+  <si>
+    <t>exp12</t>
   </si>
 </sst>
 </file>
@@ -114,14 +161,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -447,15 +500,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:M21"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:M21"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>-1.3188800000000001E-2</v>
       </c>
@@ -496,7 +590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>0.51643600000000001</v>
       </c>
@@ -537,7 +631,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>0.22340199999999999</v>
       </c>
@@ -578,7 +672,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>0.58984400000000003</v>
       </c>
@@ -619,7 +713,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1.5177299999999999E-2</v>
       </c>
@@ -660,7 +754,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1.11877</v>
       </c>
@@ -701,7 +795,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>0.766239</v>
       </c>
@@ -742,7 +836,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>0.103698</v>
       </c>
@@ -783,7 +877,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>-0.86857099999999998</v>
       </c>
@@ -824,7 +918,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>-0.66686000000000001</v>
       </c>
@@ -865,7 +959,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>-6.4713900000000005E-2</v>
       </c>
@@ -906,7 +1000,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>-0.925925</v>
       </c>
@@ -947,7 +1041,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>0.25372899999999998</v>
       </c>
@@ -988,7 +1082,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>0.322847</v>
       </c>
@@ -1029,7 +1123,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>-0.34955999999999998</v>
       </c>
@@ -1070,7 +1164,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>-0.15331400000000001</v>
       </c>
@@ -1111,7 +1205,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>-0.77882499999999999</v>
       </c>
@@ -1152,7 +1246,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>-0.54912099999999997</v>
       </c>
@@ -1193,7 +1287,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>-0.88859500000000002</v>
       </c>
@@ -1234,7 +1328,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>-2.45206E-2</v>
       </c>
@@ -1277,10 +1371,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>